<commit_message>
Fixed bounds for x_sb in constraint 2
</commit_message>
<xml_diff>
--- a/final_model/final_model.xlsx
+++ b/final_model/final_model.xlsx
@@ -5,25 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lukasobg/Documents/opiskelu/RobustBiodieselSCM/final_model/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lukasobg/Documents/kandi/RobustBiodieselSCM/final_model/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FE88AF8-844A-3841-BB89-018D280EFC6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{449CF09C-5EC6-8247-93BB-36344C6939D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="18600" windowHeight="21100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="300" yWindow="500" windowWidth="37220" windowHeight="21100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="First run" sheetId="1" r:id="rId1"/>
     <sheet name="Second run" sheetId="2" r:id="rId2"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">'Second run'!$D$15:$D$21</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">'Second run'!$P$6:$P$12</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">'Second run'!$D$15:$D$21</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">'Second run'!$P$6:$P$12</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">'Second run'!$D$15:$D$21</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">'Second run'!$P$6:$P$12</definedName>
-  </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -43,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="39">
   <si>
     <t>FINAL MODEL PARAM VALUES</t>
   </si>
@@ -443,32 +435,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <t>Total Cost (</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>obj. f. value</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>)</t>
-    </r>
-  </si>
-  <si>
     <t>Transportation Cost</t>
   </si>
   <si>
@@ -484,37 +450,7 @@
     <t>Time</t>
   </si>
   <si>
-    <t>I have the results for 300 (250 was infeasible with 3+ cap.) and 1000 suppliers, and capillarities 2,3,5,10. See excel file.</t>
-  </si>
-  <si>
-    <t>Weird or interesting things I noticed:​</t>
-  </si>
-  <si>
-    <t>-transportation cost is 99% of the total cost in all cases</t>
-  </si>
-  <si>
-    <t>-not much changes in other costs, hydrotreatment went up quite a bit with capillarity</t>
-  </si>
-  <si>
-    <t>​-when expanding capillarity:</t>
-  </si>
-  <si>
-    <t>-the amount of AF did not change at all</t>
-  </si>
-  <si>
-    <t>-proportion of AF went down</t>
-  </si>
-  <si>
-    <t>-the amount of CO went up (with the exception of 1000,2 --&gt; 1000,3 went down slightly)</t>
-  </si>
-  <si>
-    <t>-proportion of CO went down (with the exception of 1000,2 --&gt; 1000,3 went up slightly)</t>
-  </si>
-  <si>
-    <t>-proportion of PFAD went up (like we assumed in our talk)</t>
-  </si>
-  <si>
-    <t>-quality of blend not affected</t>
+    <t>Total Cost (obj, f, value)</t>
   </si>
 </sst>
 </file>
@@ -1366,15 +1302,33 @@
               </c:ext>
             </c:extLst>
           </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
           <c:cat>
             <c:strRef>
-              <c:f>('First run'!$E$11,'First run'!$G$11)</c:f>
+              <c:f>'Second run'!$E$3:$G$3</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>PFAD</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>AF</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>CO</c:v>
                 </c:pt>
               </c:strCache>
@@ -1382,16 +1336,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>('Second run'!$E$17,'Second run'!$G$17)</c:f>
+              <c:f>'Second run'!$E$17:$G$17</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>3990.2109585478702</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2975.8833352545898</c:v>
-                </c:pt>
+                <c:ptCount val="3"/>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1623,15 +1571,33 @@
               </c:ext>
             </c:extLst>
           </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
           <c:cat>
             <c:strRef>
-              <c:f>('First run'!$E$11,'First run'!$G$11)</c:f>
+              <c:f>'Second run'!$E$3:$G$3</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>PFAD</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>AF</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>CO</c:v>
                 </c:pt>
               </c:strCache>
@@ -1639,16 +1605,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>('Second run'!$E$19,'Second run'!$G$19)</c:f>
+              <c:f>'Second run'!$E$19:$G$19</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>4734.8577480135</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2906.6519842938201</c:v>
-                </c:pt>
+                <c:ptCount val="3"/>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1879,15 +1839,33 @@
               </c:ext>
             </c:extLst>
           </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
           <c:cat>
             <c:strRef>
-              <c:f>('First run'!$E$11,'First run'!$G$11)</c:f>
+              <c:f>'Second run'!$E$3:$G$3</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>PFAD</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>AF</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>CO</c:v>
                 </c:pt>
               </c:strCache>
@@ -1895,16 +1873,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>('Second run'!$E$21,'Second run'!$G$21)</c:f>
+              <c:f>'Second run'!$E$21:$G$21</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>7827.9296722576601</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>3002.1425795267101</c:v>
-                </c:pt>
+                <c:ptCount val="3"/>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -2136,15 +2108,33 @@
               </c:ext>
             </c:extLst>
           </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
           <c:cat>
             <c:strRef>
-              <c:f>('Second run'!$E$3,'Second run'!$G$3)</c:f>
+              <c:f>'Second run'!$E$3:$G$3</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>PFAD</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>AF</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>CO</c:v>
                 </c:pt>
               </c:strCache>
@@ -2152,16 +2142,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>('Second run'!$E$10,'Second run'!$G$10)</c:f>
+              <c:f>'Second run'!$E$10:$G$10</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>1198.81919634827</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>817.41341108981896</c:v>
-                </c:pt>
+                <c:ptCount val="3"/>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -2392,15 +2376,33 @@
               </c:ext>
             </c:extLst>
           </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
           <c:cat>
             <c:strRef>
-              <c:f>('Second run'!$E$3,'Second run'!$G$3)</c:f>
+              <c:f>'Second run'!$E$3:$G$3</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>PFAD</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>AF</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>CO</c:v>
                 </c:pt>
               </c:strCache>
@@ -2408,16 +2410,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>('Second run'!$E$12,'Second run'!$G$12)</c:f>
+              <c:f>'Second run'!$E$12:$G$12</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>1424.7617523133399</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>848.53835280182705</c:v>
-                </c:pt>
+                <c:ptCount val="3"/>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -2461,289 +2457,6 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr rtl="0">
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-FI"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-FI"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-FI"/>
-              <a:t>300, 2</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-FI" baseline="0"/>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-FI"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout>
-        <c:manualLayout>
-          <c:layoutTarget val="inner"/>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.15396998458220132"/>
-          <c:y val="0.13564037358592393"/>
-          <c:w val="0.7405449773323789"/>
-          <c:h val="0.67977673287407803"/>
-        </c:manualLayout>
-      </c:layout>
-      <c:pieChart>
-        <c:varyColors val="1"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:dPt>
-            <c:idx val="0"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent6"/>
-              </a:solidFill>
-              <a:ln w="19050">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000001-5139-8A40-A997-27724DAFFF57}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="1"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent5"/>
-              </a:solidFill>
-              <a:ln w="19050">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000003-5139-8A40-A997-27724DAFFF57}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="2"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
-              <a:ln w="19050">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000005-94D4-A645-9A14-086DC3229EA5}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
-          <c:cat>
-            <c:strRef>
-              <c:f>'First run'!$E$11:$G$11</c:f>
-              <c:strCache>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>PFAD</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>AF</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>CO</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Second run'!$E$6:$G$6</c:f>
-              <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>955.28457213964396</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1064.52999999999</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>778.96969011835802</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000004-5139-8A40-A997-27724DAFFF57}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-          <c:showLeaderLines val="1"/>
-        </c:dLbls>
-        <c:firstSliceAng val="0"/>
-      </c:pieChart>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
             <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
@@ -4422,15 +4135,33 @@
               </c:ext>
             </c:extLst>
           </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
           <c:cat>
             <c:strRef>
-              <c:f>('First run'!$E$11,'First run'!$G$11)</c:f>
+              <c:f>'Second run'!$E$3:$G$3</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>PFAD</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>AF</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>CO</c:v>
                 </c:pt>
               </c:strCache>
@@ -4438,16 +4169,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>('Second run'!$E$6,'Second run'!$G$6)</c:f>
+              <c:f>'Second run'!$E$6:$G$6</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>955.28457213964396</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>778.96969011835802</c:v>
-                </c:pt>
+                <c:ptCount val="3"/>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -4679,15 +4404,33 @@
               </c:ext>
             </c:extLst>
           </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
           <c:cat>
             <c:strRef>
-              <c:f>('First run'!$E$11,'First run'!$G$11)</c:f>
+              <c:f>'Second run'!$E$3:$G$3</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>PFAD</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>AF</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>CO</c:v>
                 </c:pt>
               </c:strCache>
@@ -4695,16 +4438,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>('Second run'!$E$8,'Second run'!$G$8)</c:f>
+              <c:f>'Second run'!$E$8:$G$8</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>1076.4282671332301</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>796.70809020255399</c:v>
-                </c:pt>
+                <c:ptCount val="3"/>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -4936,15 +4673,33 @@
               </c:ext>
             </c:extLst>
           </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
           <c:cat>
             <c:strRef>
-              <c:f>('First run'!$E$11,'First run'!$G$11)</c:f>
+              <c:f>'Second run'!$E$3:$G$3</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>PFAD</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>AF</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>CO</c:v>
                 </c:pt>
               </c:strCache>
@@ -4952,16 +4707,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>('Second run'!$E$15,'Second run'!$G$15)</c:f>
+              <c:f>'Second run'!$E$15:$G$15</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>3517.77118130811</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2779.87604679588</c:v>
-                </c:pt>
+                <c:ptCount val="3"/>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -5251,43 +5000,6 @@
 </file>
 
 <file path=xl/charts/colors14.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="13">
-  <a:schemeClr val="accent6"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent4"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
-<file path=xl/charts/colors15.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="13">
   <a:schemeClr val="accent6"/>
   <a:schemeClr val="accent5"/>
@@ -8219,525 +7931,6 @@
 </file>
 
 <file path=xl/charts/style14.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="251">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050">
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="25400">
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/charts/style15.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="251">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -13927,44 +13120,6 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>59393</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>188925</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>678900</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>52278</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="20" name="Chart 19">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000014000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks/>
-        </xdr:cNvGraphicFramePr>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId9"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -14737,10 +13892,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1B044A6-1D3E-2B41-96E0-31015096A347}">
-  <dimension ref="A1:X75"/>
+  <dimension ref="A1:X63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q15" sqref="Q15"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -14835,7 +13990,7 @@
     <row r="4" spans="1:24" ht="49" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="23"/>
       <c r="B4" s="25" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C4" s="25" t="s">
         <v>6</v>
@@ -14865,19 +14020,19 @@
         <v>32</v>
       </c>
       <c r="L4" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="M4" s="35" t="s">
+        <v>33</v>
+      </c>
+      <c r="N4" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="N4" s="25" t="s">
+      <c r="O4" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="O4" s="25" t="s">
-        <v>36</v>
-      </c>
       <c r="P4" s="25" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="T4" s="23"/>
       <c r="U4" s="23"/>
@@ -14910,52 +14065,21 @@
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A6" s="23"/>
-      <c r="B6" s="48">
-        <v>0.24</v>
-      </c>
-      <c r="C6" s="48">
-        <v>300</v>
-      </c>
-      <c r="D6" s="49">
-        <v>2</v>
-      </c>
-      <c r="E6" s="56">
-        <v>955.28457213964396</v>
-      </c>
-      <c r="F6" s="56">
-        <v>1064.52999999999</v>
-      </c>
-      <c r="G6" s="56">
-        <v>778.96969011835802</v>
-      </c>
-      <c r="H6" s="57">
-        <v>2798.7842622580001</v>
-      </c>
-      <c r="I6" s="56">
-        <v>2518.9310560436002</v>
-      </c>
-      <c r="J6" s="57">
-        <v>1500</v>
-      </c>
-      <c r="K6" s="58">
-        <v>0.89833036953033096</v>
-      </c>
-      <c r="L6" s="56">
-        <v>293379.32932461699</v>
-      </c>
-      <c r="M6" s="56">
-        <v>189575649.96575201</v>
-      </c>
-      <c r="N6" s="56">
-        <v>141031.667391503</v>
-      </c>
-      <c r="O6" s="56">
-        <v>267971.38894080801</v>
-      </c>
-      <c r="P6" s="59">
-        <f>SUM(L6:O6)</f>
-        <v>190278032.35140893</v>
-      </c>
+      <c r="B6" s="48"/>
+      <c r="C6" s="48"/>
+      <c r="D6" s="49"/>
+      <c r="E6" s="56"/>
+      <c r="F6" s="56"/>
+      <c r="G6" s="56"/>
+      <c r="H6" s="57"/>
+      <c r="I6" s="56"/>
+      <c r="J6" s="57"/>
+      <c r="K6" s="58"/>
+      <c r="L6" s="56"/>
+      <c r="M6" s="56"/>
+      <c r="N6" s="56"/>
+      <c r="O6" s="56"/>
+      <c r="P6" s="59"/>
       <c r="T6" s="23"/>
       <c r="U6" s="23"/>
       <c r="V6" s="23"/>
@@ -14965,37 +14089,38 @@
     <row r="7" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A7" s="23"/>
       <c r="D7" s="41"/>
-      <c r="E7" s="54">
+      <c r="E7" s="54" t="e">
         <f>E6/H6</f>
-        <v>0.34132126045647426</v>
-      </c>
-      <c r="F7" s="54">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F7" s="54" t="e">
         <f>F6/H6</f>
-        <v>0.38035443258536461</v>
-      </c>
-      <c r="G7" s="54">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G7" s="54" t="e">
         <f>G6/H6</f>
-        <v>0.27832430695815824</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="H7" s="42"/>
       <c r="J7" s="42"/>
       <c r="K7" s="43"/>
-      <c r="L7" s="55">
+      <c r="L7" s="55" t="e">
         <f>L6/P6</f>
-        <v>1.541845507330025E-3</v>
-      </c>
-      <c r="M7" s="55">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M7" s="55" t="e">
         <f>M6/P6</f>
-        <v>0.99630865225492904</v>
-      </c>
-      <c r="N7" s="55">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N7" s="55" t="e">
         <f>N6/P6</f>
-        <v>7.4118733333884365E-4</v>
-      </c>
-      <c r="O7" s="54">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O7" s="54" t="e">
         <f>O6/P6</f>
-        <v>1.4083149044021729E-3</v>
-      </c>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P7" s="59"/>
       <c r="T7" s="23"/>
       <c r="U7" s="23"/>
       <c r="V7" s="23"/>
@@ -15004,52 +14129,21 @@
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A8" s="23"/>
-      <c r="B8" s="48">
-        <v>0.25</v>
-      </c>
-      <c r="C8" s="48">
-        <v>300</v>
-      </c>
-      <c r="D8" s="49">
-        <v>3</v>
-      </c>
-      <c r="E8" s="50">
-        <v>1076.4282671332301</v>
-      </c>
-      <c r="F8" s="50">
-        <v>1064.52999999999</v>
-      </c>
-      <c r="G8" s="50">
-        <v>796.70809020255399</v>
-      </c>
-      <c r="H8" s="51">
-        <v>2937.66635733578</v>
-      </c>
-      <c r="I8" s="50">
-        <v>2646.2022781860901</v>
-      </c>
-      <c r="J8" s="51">
-        <v>1500</v>
-      </c>
-      <c r="K8" s="52">
-        <v>0.89873993074527603</v>
-      </c>
-      <c r="L8" s="50">
-        <v>307090.154831552</v>
-      </c>
-      <c r="M8" s="50">
-        <v>205237195.44226101</v>
-      </c>
-      <c r="N8" s="50">
-        <v>146764.33519545599</v>
-      </c>
-      <c r="O8" s="50">
-        <v>281510.880658095</v>
-      </c>
-      <c r="P8" s="44">
-        <f>SUM(L8:O8)</f>
-        <v>205972560.81294611</v>
-      </c>
+      <c r="B8" s="48"/>
+      <c r="C8" s="48"/>
+      <c r="D8" s="49"/>
+      <c r="E8" s="50"/>
+      <c r="F8" s="50"/>
+      <c r="G8" s="50"/>
+      <c r="H8" s="51"/>
+      <c r="I8" s="50"/>
+      <c r="J8" s="51"/>
+      <c r="K8" s="52"/>
+      <c r="L8" s="50"/>
+      <c r="M8" s="50"/>
+      <c r="N8" s="50"/>
+      <c r="O8" s="50"/>
+      <c r="P8" s="59"/>
       <c r="T8" s="23"/>
       <c r="U8" s="23"/>
       <c r="V8" s="23"/>
@@ -15059,91 +14153,61 @@
     <row r="9" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A9" s="23"/>
       <c r="D9" s="41"/>
-      <c r="E9" s="54">
+      <c r="E9" s="54" t="e">
         <f>E8/H8</f>
-        <v>0.36642291404033417</v>
-      </c>
-      <c r="F9" s="54">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F9" s="54" t="e">
         <f>F8/H8</f>
-        <v>0.36237266949723673</v>
-      </c>
-      <c r="G9" s="54">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G9" s="54" t="e">
         <f>G8/H8</f>
-        <v>0.27120441646242704</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="H9" s="42"/>
       <c r="J9" s="42"/>
       <c r="K9" s="43"/>
-      <c r="L9" s="55">
+      <c r="L9" s="55" t="e">
         <f>L8/P8</f>
-        <v>1.4909274983983705E-3</v>
-      </c>
-      <c r="M9" s="55">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M9" s="55" t="e">
         <f>M8/P8</f>
-        <v>0.99642978963905326</v>
-      </c>
-      <c r="N9" s="55">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N9" s="55" t="e">
         <f>N8/P8</f>
-        <v>7.1254313980559749E-4</v>
-      </c>
-      <c r="O9" s="54">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O9" s="54" t="e">
         <f>O8/P8</f>
-        <v>1.3667397227427249E-3</v>
-      </c>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P9" s="59"/>
       <c r="T9" s="23"/>
       <c r="U9" s="23"/>
       <c r="V9" s="23"/>
       <c r="W9" s="23"/>
       <c r="X9" s="23"/>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="23"/>
-      <c r="B10" s="31">
-        <v>0.24</v>
-      </c>
-      <c r="C10" s="31">
-        <v>300</v>
-      </c>
-      <c r="D10" s="32">
-        <v>5</v>
-      </c>
-      <c r="E10" s="44">
-        <v>1198.81919634827</v>
-      </c>
-      <c r="F10" s="44">
-        <v>1064.52999999999</v>
-      </c>
-      <c r="G10" s="44">
-        <v>817.41341108981896</v>
-      </c>
-      <c r="H10" s="45">
-        <v>3080.7626074380901</v>
-      </c>
-      <c r="I10" s="44">
-        <v>2777.2440237149699</v>
-      </c>
-      <c r="J10" s="45">
-        <v>1500</v>
-      </c>
-      <c r="K10" s="46">
-        <v>0.89907903659806898</v>
-      </c>
-      <c r="L10" s="47">
-        <v>321192.72663291002</v>
-      </c>
-      <c r="M10" s="44">
-        <v>221112534.963433</v>
-      </c>
-      <c r="N10" s="44">
-        <v>152695.23840842201</v>
-      </c>
-      <c r="O10" s="44">
-        <v>295451.49188457202</v>
-      </c>
-      <c r="P10" s="44">
-        <f>SUM(L10:O10)</f>
-        <v>221881874.4203589</v>
-      </c>
+      <c r="B10" s="31"/>
+      <c r="C10" s="31"/>
+      <c r="D10" s="32"/>
+      <c r="E10" s="44"/>
+      <c r="F10" s="44"/>
+      <c r="G10" s="44"/>
+      <c r="H10" s="45"/>
+      <c r="I10" s="44"/>
+      <c r="J10" s="45"/>
+      <c r="K10" s="46"/>
+      <c r="L10" s="47"/>
+      <c r="M10" s="44"/>
+      <c r="N10" s="44"/>
+      <c r="O10" s="44"/>
+      <c r="P10" s="59"/>
       <c r="T10" s="23"/>
       <c r="U10" s="23"/>
       <c r="V10" s="23"/>
@@ -15153,91 +14217,61 @@
     <row r="11" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A11" s="23"/>
       <c r="D11" s="41"/>
-      <c r="E11" s="54">
+      <c r="E11" s="54" t="e">
         <f>E10/H10</f>
-        <v>0.38913066312019012</v>
-      </c>
-      <c r="F11" s="54">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F11" s="54" t="e">
         <f>F10/H10</f>
-        <v>0.34554106747135416</v>
-      </c>
-      <c r="G11" s="54">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G11" s="54" t="e">
         <f>G10/H10</f>
-        <v>0.26532826940845211</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="H11" s="42"/>
       <c r="J11" s="42"/>
       <c r="K11" s="43"/>
-      <c r="L11" s="55">
+      <c r="L11" s="55" t="e">
         <f>L10/P10</f>
-        <v>1.4475843395139391E-3</v>
-      </c>
-      <c r="M11" s="55">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M11" s="55" t="e">
         <f>M10/P10</f>
-        <v>0.99653266198991819</v>
-      </c>
-      <c r="N11" s="55">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N11" s="55" t="e">
         <f>N10/P10</f>
-        <v>6.8818256924915982E-4</v>
-      </c>
-      <c r="O11" s="54">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O11" s="54" t="e">
         <f>O10/P10</f>
-        <v>1.3315711013186875E-3</v>
-      </c>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P11" s="59"/>
       <c r="T11" s="23"/>
       <c r="U11" s="23"/>
       <c r="V11" s="23"/>
       <c r="W11" s="23"/>
       <c r="X11" s="23"/>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:24" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="23"/>
-      <c r="B12" s="31">
-        <v>0.49</v>
-      </c>
-      <c r="C12" s="31">
-        <v>300</v>
-      </c>
-      <c r="D12" s="32">
-        <v>10</v>
-      </c>
-      <c r="E12" s="44">
-        <v>1424.7617523133399</v>
-      </c>
-      <c r="F12" s="44">
-        <v>1064.52999999999</v>
-      </c>
-      <c r="G12" s="44">
-        <v>848.53835280182705</v>
-      </c>
-      <c r="H12" s="45">
-        <v>3337.8301051151702</v>
-      </c>
-      <c r="I12" s="44">
-        <v>3012.8843047667301</v>
-      </c>
-      <c r="J12" s="45">
-        <v>1500</v>
-      </c>
-      <c r="K12" s="46">
-        <v>0.89730766525120997</v>
-      </c>
-      <c r="L12" s="47">
-        <v>346588.2269835</v>
-      </c>
-      <c r="M12" s="44">
-        <v>255316295.56066599</v>
-      </c>
-      <c r="N12" s="44">
-        <v>163289.187732625</v>
-      </c>
-      <c r="O12" s="44">
-        <v>320519.606890077</v>
-      </c>
-      <c r="P12" s="44">
-        <f>SUM(L12:O12)</f>
-        <v>256146692.5822722</v>
-      </c>
+      <c r="B12" s="31"/>
+      <c r="C12" s="31"/>
+      <c r="D12" s="32"/>
+      <c r="E12" s="44"/>
+      <c r="F12" s="44"/>
+      <c r="G12" s="44"/>
+      <c r="H12" s="45"/>
+      <c r="I12" s="44"/>
+      <c r="J12" s="45"/>
+      <c r="K12" s="46"/>
+      <c r="L12" s="47"/>
+      <c r="M12" s="44"/>
+      <c r="N12" s="44"/>
+      <c r="O12" s="44"/>
+      <c r="P12" s="59"/>
       <c r="T12" s="23"/>
       <c r="U12" s="23"/>
       <c r="V12" s="23"/>
@@ -15249,39 +14283,39 @@
       <c r="B13" s="31"/>
       <c r="C13" s="31"/>
       <c r="D13" s="32"/>
-      <c r="E13" s="54">
+      <c r="E13" s="54" t="e">
         <f>E12/H12</f>
-        <v>0.42685268795733966</v>
-      </c>
-      <c r="F13" s="54">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F13" s="54" t="e">
         <f>F12/H12</f>
-        <v>0.31892875505215651</v>
-      </c>
-      <c r="G13" s="54">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G13" s="54" t="e">
         <f>G12/H12</f>
-        <v>0.25421855699049989</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="H13" s="45"/>
       <c r="I13" s="44"/>
       <c r="J13" s="45"/>
       <c r="K13" s="46"/>
-      <c r="L13" s="55">
+      <c r="L13" s="55" t="e">
         <f>L12/P12</f>
-        <v>1.3530849197757209E-3</v>
-      </c>
-      <c r="M13" s="55">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M13" s="55" t="e">
         <f>M12/P12</f>
-        <v>0.99675811929002567</v>
-      </c>
-      <c r="N13" s="55">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N13" s="55" t="e">
         <f>N12/P12</f>
-        <v>6.3748310035343465E-4</v>
-      </c>
-      <c r="O13" s="54">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O13" s="54" t="e">
         <f>O12/P12</f>
-        <v>1.2513126898452095E-3</v>
-      </c>
-      <c r="P13" s="44"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P13" s="59"/>
       <c r="T13" s="23"/>
       <c r="U13" s="23"/>
       <c r="V13" s="23"/>
@@ -15302,52 +14336,21 @@
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A15" s="23"/>
-      <c r="B15" s="31">
-        <v>1.54</v>
-      </c>
-      <c r="C15" s="31">
-        <v>1000</v>
-      </c>
-      <c r="D15" s="32">
-        <v>2</v>
-      </c>
-      <c r="E15" s="44">
-        <v>3517.77118130811</v>
-      </c>
-      <c r="F15" s="44">
-        <v>3504.54</v>
-      </c>
-      <c r="G15" s="44">
-        <v>2779.87604679588</v>
-      </c>
-      <c r="H15" s="45">
-        <v>9802.1872281039905</v>
-      </c>
-      <c r="I15" s="44">
-        <v>8826.4235071699204</v>
-      </c>
-      <c r="J15" s="45">
-        <v>1500</v>
-      </c>
-      <c r="K15" s="46">
-        <v>0.9</v>
-      </c>
-      <c r="L15" s="47">
-        <v>1022510.76234243</v>
-      </c>
-      <c r="M15" s="44">
-        <v>656580341.91927898</v>
-      </c>
-      <c r="N15" s="44">
-        <v>489977.04959211801</v>
-      </c>
-      <c r="O15" s="44">
-        <v>938981.22416701296</v>
-      </c>
-      <c r="P15" s="44">
-        <f>SUM(L15:O15)</f>
-        <v>659031810.95538056</v>
-      </c>
+      <c r="B15" s="31"/>
+      <c r="C15" s="31"/>
+      <c r="D15" s="32"/>
+      <c r="E15" s="44"/>
+      <c r="F15" s="44"/>
+      <c r="G15" s="44"/>
+      <c r="H15" s="45"/>
+      <c r="I15" s="44"/>
+      <c r="J15" s="45"/>
+      <c r="K15" s="46"/>
+      <c r="L15" s="47"/>
+      <c r="M15" s="44"/>
+      <c r="N15" s="44"/>
+      <c r="O15" s="44"/>
+      <c r="P15" s="44"/>
       <c r="T15" s="23"/>
       <c r="U15" s="23"/>
       <c r="V15" s="23"/>
@@ -15357,36 +14360,36 @@
     <row r="16" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A16" s="23"/>
       <c r="D16" s="41"/>
-      <c r="E16" s="54">
+      <c r="E16" s="54" t="e">
         <f>E15/H15</f>
-        <v>0.35887614666472173</v>
-      </c>
-      <c r="F16" s="54">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F16" s="54" t="e">
         <f>F15/H15</f>
-        <v>0.35752632738457429</v>
-      </c>
-      <c r="G16" s="54">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G16" s="54" t="e">
         <f>G15/H15</f>
-        <v>0.28359752595070392</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="H16" s="42"/>
       <c r="J16" s="42"/>
       <c r="K16" s="43"/>
-      <c r="L16" s="55">
+      <c r="L16" s="55" t="e">
         <f>L15/P15</f>
-        <v>1.5515347595438888E-3</v>
-      </c>
-      <c r="M16" s="55">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M16" s="55" t="e">
         <f>M15/P15</f>
-        <v>0.99628019619789254</v>
-      </c>
-      <c r="N16" s="55">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N16" s="55" t="e">
         <f>N15/P15</f>
-        <v>7.4348011954356431E-4</v>
-      </c>
-      <c r="O16" s="54">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O16" s="54" t="e">
         <f>O15/P15</f>
-        <v>1.4247889230199636E-3</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="T16" s="23"/>
       <c r="U16" s="23"/>
@@ -15397,49 +14400,20 @@
     <row r="17" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A17" s="23"/>
       <c r="B17" s="31"/>
-      <c r="C17" s="33">
-        <v>1000</v>
-      </c>
-      <c r="D17" s="32">
-        <v>3</v>
-      </c>
-      <c r="E17" s="44">
-        <v>3990.2109585478702</v>
-      </c>
-      <c r="F17" s="44">
-        <v>3504.54</v>
-      </c>
-      <c r="G17" s="44">
-        <v>2975.8833352545898</v>
-      </c>
-      <c r="H17" s="45">
-        <v>10470.634293802401</v>
-      </c>
-      <c r="I17" s="44">
-        <v>9434.8270700452595</v>
-      </c>
-      <c r="J17" s="45">
-        <v>1500</v>
-      </c>
-      <c r="K17" s="46">
-        <v>0.9</v>
-      </c>
-      <c r="L17" s="47">
-        <v>1087395.3960277</v>
-      </c>
-      <c r="M17" s="44">
-        <v>721733854.77226996</v>
-      </c>
-      <c r="N17" s="44">
-        <v>518675.00510464498</v>
-      </c>
-      <c r="O17" s="44">
-        <v>1003705.00745162</v>
-      </c>
-      <c r="P17" s="44">
-        <f>SUM(L17:O17)</f>
-        <v>724343630.18085396</v>
-      </c>
+      <c r="C17" s="33"/>
+      <c r="D17" s="32"/>
+      <c r="E17" s="44"/>
+      <c r="F17" s="44"/>
+      <c r="G17" s="44"/>
+      <c r="H17" s="45"/>
+      <c r="I17" s="44"/>
+      <c r="J17" s="45"/>
+      <c r="K17" s="46"/>
+      <c r="L17" s="47"/>
+      <c r="M17" s="44"/>
+      <c r="N17" s="44"/>
+      <c r="O17" s="44"/>
+      <c r="P17" s="44"/>
       <c r="T17" s="23"/>
       <c r="U17" s="23"/>
       <c r="V17" s="23"/>
@@ -15449,36 +14423,36 @@
     <row r="18" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A18" s="23"/>
       <c r="D18" s="41"/>
-      <c r="E18" s="54">
+      <c r="E18" s="54" t="e">
         <f>E17/H17</f>
-        <v>0.38108588711857577</v>
-      </c>
-      <c r="F18" s="54">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F18" s="54" t="e">
         <f>F17/H17</f>
-        <v>0.33470178612525386</v>
-      </c>
-      <c r="G18" s="54">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G18" s="54" t="e">
         <f>G17/H17</f>
-        <v>0.28421232675617597</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="H18" s="42"/>
       <c r="J18" s="42"/>
       <c r="K18" s="43"/>
-      <c r="L18" s="55">
+      <c r="L18" s="55" t="e">
         <f>L17/P17</f>
-        <v>1.5012148250081242E-3</v>
-      </c>
-      <c r="M18" s="55">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M18" s="55" t="e">
         <f>M17/P17</f>
-        <v>0.99639704789295602</v>
-      </c>
-      <c r="N18" s="55">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N18" s="55" t="e">
         <f>N17/P17</f>
-        <v>7.1606207812601635E-4</v>
-      </c>
-      <c r="O18" s="54">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O18" s="54" t="e">
         <f>O17/P17</f>
-        <v>1.3856752039098006E-3</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="T18" s="23"/>
       <c r="U18" s="23"/>
@@ -15488,52 +14462,21 @@
     </row>
     <row r="19" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A19" s="23"/>
-      <c r="B19" s="31">
-        <v>4.22</v>
-      </c>
-      <c r="C19" s="31">
-        <v>1000</v>
-      </c>
-      <c r="D19" s="32">
-        <v>5</v>
-      </c>
-      <c r="E19" s="44">
-        <v>4734.8577480135</v>
-      </c>
-      <c r="F19" s="44">
-        <v>3504.54</v>
-      </c>
-      <c r="G19" s="44">
-        <v>2906.6519842938201</v>
-      </c>
-      <c r="H19" s="45">
-        <v>11146.0497323073</v>
-      </c>
-      <c r="I19" s="44">
-        <v>10059.622870792</v>
-      </c>
-      <c r="J19" s="45">
-        <v>1500</v>
-      </c>
-      <c r="K19" s="46">
-        <v>0.9</v>
-      </c>
-      <c r="L19" s="47">
-        <v>1155629.2533877899</v>
-      </c>
-      <c r="M19" s="44">
-        <v>816261886.49899197</v>
-      </c>
-      <c r="N19" s="44">
-        <v>544999.309135227</v>
-      </c>
-      <c r="O19" s="44">
-        <v>1070172.64582894</v>
-      </c>
-      <c r="P19" s="44">
-        <f>SUM(L19:O19)</f>
-        <v>819032687.70734394</v>
-      </c>
+      <c r="B19" s="31"/>
+      <c r="C19" s="31"/>
+      <c r="D19" s="32"/>
+      <c r="E19" s="44"/>
+      <c r="F19" s="44"/>
+      <c r="G19" s="44"/>
+      <c r="H19" s="45"/>
+      <c r="I19" s="44"/>
+      <c r="J19" s="45"/>
+      <c r="K19" s="46"/>
+      <c r="L19" s="47"/>
+      <c r="M19" s="44"/>
+      <c r="N19" s="44"/>
+      <c r="O19" s="44"/>
+      <c r="P19" s="44"/>
       <c r="T19" s="23"/>
       <c r="U19" s="23"/>
       <c r="V19" s="23"/>
@@ -15543,36 +14486,36 @@
     <row r="20" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A20" s="23"/>
       <c r="D20" s="41"/>
-      <c r="E20" s="54">
+      <c r="E20" s="54" t="e">
         <f>E19/H19</f>
-        <v>0.42480141949208367</v>
-      </c>
-      <c r="F20" s="54">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F20" s="54" t="e">
         <f>F19/H19</f>
-        <v>0.31441991415505188</v>
-      </c>
-      <c r="G20" s="54">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G20" s="54" t="e">
         <f>G19/H19</f>
-        <v>0.26077866635286628</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="H20" s="42"/>
       <c r="J20" s="42"/>
       <c r="K20" s="43"/>
-      <c r="L20" s="55">
+      <c r="L20" s="55" t="e">
         <f>L19/P19</f>
-        <v>1.4109684152199776E-3</v>
-      </c>
-      <c r="M20" s="55">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M20" s="55" t="e">
         <f>M19/P19</f>
-        <v>0.99661698336349913</v>
-      </c>
-      <c r="N20" s="55">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N20" s="55" t="e">
         <f>N19/P19</f>
-        <v>6.6541826390446293E-4</v>
-      </c>
-      <c r="O20" s="54">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O20" s="54" t="e">
         <f>O19/P19</f>
-        <v>1.3066299573764181E-3</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="T20" s="23"/>
       <c r="U20" s="23"/>
@@ -15582,52 +14525,21 @@
     </row>
     <row r="21" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A21" s="23"/>
-      <c r="B21" s="31">
-        <v>26.7</v>
-      </c>
-      <c r="C21" s="31">
-        <v>1000</v>
-      </c>
-      <c r="D21" s="32">
-        <v>10</v>
-      </c>
-      <c r="E21" s="44">
-        <v>7827.9296722576601</v>
-      </c>
-      <c r="F21" s="44">
-        <v>3504.54</v>
-      </c>
-      <c r="G21" s="44">
-        <v>3002.1425795267101</v>
-      </c>
-      <c r="H21" s="45">
-        <v>14334.6122517843</v>
-      </c>
-      <c r="I21" s="44">
-        <v>12993.336217353501</v>
-      </c>
-      <c r="J21" s="45">
-        <v>1500</v>
-      </c>
-      <c r="K21" s="46">
-        <v>0.9</v>
-      </c>
-      <c r="L21" s="47">
-        <v>1473530.59938317</v>
-      </c>
-      <c r="M21" s="44">
-        <v>1223999724.94067</v>
-      </c>
-      <c r="N21" s="44">
-        <v>673496.71586664603</v>
-      </c>
-      <c r="O21" s="44">
-        <v>1382269.8103567599</v>
-      </c>
-      <c r="P21" s="44">
-        <f>SUM(L21:O21)</f>
-        <v>1227529022.0662766</v>
-      </c>
+      <c r="B21" s="31"/>
+      <c r="C21" s="31"/>
+      <c r="D21" s="32"/>
+      <c r="E21" s="44"/>
+      <c r="F21" s="44"/>
+      <c r="G21" s="44"/>
+      <c r="H21" s="45"/>
+      <c r="I21" s="44"/>
+      <c r="J21" s="45"/>
+      <c r="K21" s="46"/>
+      <c r="L21" s="47"/>
+      <c r="M21" s="44"/>
+      <c r="N21" s="44"/>
+      <c r="O21" s="44"/>
+      <c r="P21" s="44"/>
       <c r="T21" s="23"/>
       <c r="U21" s="23"/>
       <c r="V21" s="23"/>
@@ -15636,33 +14548,33 @@
     </row>
     <row r="22" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A22" s="23"/>
-      <c r="E22" s="54">
+      <c r="E22" s="54" t="e">
         <f>E21/H21</f>
-        <v>0.5460859027619166</v>
-      </c>
-      <c r="F22" s="54">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F22" s="54" t="e">
         <f>F21/H21</f>
-        <v>0.24448097642569805</v>
-      </c>
-      <c r="G22" s="54">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G22" s="54" t="e">
         <f>G21/H21</f>
-        <v>0.20943312081239021</v>
-      </c>
-      <c r="L22" s="55">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L22" s="55" t="e">
         <f>L21/P21</f>
-        <v>1.2004038787635373E-3</v>
-      </c>
-      <c r="M22" s="55">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M22" s="55" t="e">
         <f>M21/P21</f>
-        <v>0.99712487683617801</v>
-      </c>
-      <c r="N22" s="55">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N22" s="55" t="e">
         <f>N21/P21</f>
-        <v>5.4866052350677761E-4</v>
-      </c>
-      <c r="O22" s="54">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O22" s="54" t="e">
         <f>O21/P21</f>
-        <v>1.1260587615517319E-3</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="T22" s="23"/>
       <c r="U22" s="23"/>
@@ -16247,60 +15159,8 @@
       <c r="W45" s="23"/>
       <c r="X45" s="23"/>
     </row>
-    <row r="52" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C52" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="55" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C55" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="58" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C58" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="60" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C60" t="s">
-        <v>42</v>
-      </c>
-    </row>
     <row r="63" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C63" s="60" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="65" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C65" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="67" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C67" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="69" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C69" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="71" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C71" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="73" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C73" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="75" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C75" t="s">
-        <v>49</v>
-      </c>
+      <c r="C63" s="60"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>